<commit_message>
feat: fixing some strategy
</commit_message>
<xml_diff>
--- a/closed_positions_pnl.xlsx
+++ b/closed_positions_pnl.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,32 +472,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DOTUSDT</t>
+          <t>1000PEPEUSDT</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-04-12 19:22:22</t>
+          <t>2025-04-12 17:59:49</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SHORT</t>
+          <t>LONG</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>-0.35532355</v>
+        <v>-1.26180085</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AXSUSDT</t>
+          <t>BTCUSDT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-04-12 19:16:23</t>
+          <t>2025-04-12 18:55:04</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -505,19 +505,19 @@
           <t>SHORT</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>-0.44238786</v>
+      <c r="D3" s="3" t="n">
+        <v>0.62730231</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ETCUSDT</t>
+          <t>LTCUSDT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-04-12 19:02:11</t>
+          <t>2025-04-12 18:55:44</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -525,19 +525,19 @@
           <t>SHORT</t>
         </is>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>-0.3900482</v>
+      <c r="D4" s="3" t="n">
+        <v>0.9244540999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>LTCUSDT</t>
+          <t>ETCUSDT</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-04-12 18:55:44</t>
+          <t>2025-04-12 19:02:11</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -545,19 +545,19 @@
           <t>SHORT</t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
-        <v>0.9244540999999999</v>
+      <c r="D5" s="2" t="n">
+        <v>-0.3900482</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BTCUSDT</t>
+          <t>AXSUSDT</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-04-12 18:55:04</t>
+          <t>2025-04-12 19:16:23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -565,28 +565,28 @@
           <t>SHORT</t>
         </is>
       </c>
-      <c r="D6" s="3" t="n">
-        <v>0.62730231</v>
+      <c r="D6" s="2" t="n">
+        <v>-0.44238786</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1000PEPEUSDT</t>
+          <t>DOTUSDT</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-04-12 17:59:49</t>
+          <t>2025-04-12 19:22:22</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>LONG</t>
+          <t>SHORT</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>-1.26180085</v>
+        <v>-0.35532355</v>
       </c>
     </row>
     <row r="8">
@@ -712,12 +712,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BNBUSDT</t>
+          <t>AVAXUSDT</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-04-13 07:31:52</t>
+          <t>2025-04-13 07:18:14</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -726,18 +726,18 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>-0.9735372</v>
+        <v>-0.56489303</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>FILUSDT</t>
+          <t>GALAUSDT</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-04-13 07:28:25</t>
+          <t>2025-04-13 07:28:06</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -746,18 +746,18 @@
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>-1.01485802</v>
+        <v>-0.80833973</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GALAUSDT</t>
+          <t>FILUSDT</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-04-13 07:28:06</t>
+          <t>2025-04-13 07:28:25</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -766,18 +766,18 @@
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>-0.80833973</v>
+        <v>-1.01485802</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>AVAXUSDT</t>
+          <t>BNBUSDT</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-04-13 07:18:14</t>
+          <t>2025-04-13 07:31:52</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -786,7 +786,7 @@
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>-0.56489303</v>
+        <v>-0.9735372</v>
       </c>
     </row>
     <row r="18">
@@ -812,12 +812,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SEIUSDT</t>
+          <t>ARBUSDT</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-04-13 16:05:41</t>
+          <t>2025-04-13 16:04:47</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -825,8 +825,8 @@
           <t>SHORT</t>
         </is>
       </c>
-      <c r="D19" s="2" t="n">
-        <v>-0.90013508</v>
+      <c r="D19" s="3" t="n">
+        <v>0.08031737999999999</v>
       </c>
     </row>
     <row r="20">
@@ -852,12 +852,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ARBUSDT</t>
+          <t>SEIUSDT</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-04-13 16:04:47</t>
+          <t>2025-04-13 16:05:41</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -865,8 +865,8 @@
           <t>SHORT</t>
         </is>
       </c>
-      <c r="D21" s="3" t="n">
-        <v>0.08031737999999999</v>
+      <c r="D21" s="2" t="n">
+        <v>-0.90013508</v>
       </c>
     </row>
     <row r="22">
@@ -887,6 +887,246 @@
       </c>
       <c r="D22" s="3" t="n">
         <v>0.04400413</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>WLDUSDT</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-04-26 17:28:45</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>-3.66210333</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>POPCATUSDT</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-04-26 19:57:55</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>5.21158425</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ETHUSDT</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-04-27 08:18:14</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>5.34782553</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>POPCATUSDT</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-04-28 12:43:07</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>0.7938678</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>AKTUSDT</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-05-01 06:48:20</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>-3.17411625</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ETHUSDT</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-05-02 12:30:07</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>8.23921752</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>SOLUSDT</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-05-02 21:49:15</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>-5.4093149</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1000PEPEUSDT</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-05-02 21:49:40</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>-4.2750705</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>POPCATUSDT</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2025-05-04 05:30:55</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>10.21847556</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>LINKUSDT</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2025-05-04 00:48:02</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>-5.9322166</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>SUIUSDT</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-05-03 07:19:57</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>9.467715200000001</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>SUIUSDT</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2025-05-03 00:40:47</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>-5.65980602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>